<commit_message>
Add sapling rate control.
</commit_message>
<xml_diff>
--- a/doc/NBV2_GPIO.xlsx
+++ b/doc/NBV2_GPIO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/971f4268de3e2582/科研要紧/NickelBird/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="411" documentId="13_ncr:1_{D48D8279-D192-4022-8AA3-94D21E562998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D886E1D-9A7C-4B5D-8E92-2373CF910927}"/>
+  <xr:revisionPtr revIDLastSave="412" documentId="13_ncr:1_{D48D8279-D192-4022-8AA3-94D21E562998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1E7F73B-5567-48EA-9E8E-D1B4F85A167F}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="7965" windowWidth="21840" windowHeight="13020" firstSheet="1" activeTab="2" xr2:uid="{9B99CC55-A333-4B3D-AAE7-60B2FBD2224A}"/>
+    <workbookView xWindow="-21720" yWindow="7965" windowWidth="21840" windowHeight="13020" firstSheet="1" activeTab="1" xr2:uid="{9B99CC55-A333-4B3D-AAE7-60B2FBD2224A}"/>
   </bookViews>
   <sheets>
     <sheet name="F405VG" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="388">
   <si>
     <t>Pin</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -1696,7 +1696,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1718,9 +1718,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="差" xfId="1" builtinId="27"/>
@@ -1739,10 +1736,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4053,8 +4046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5260BC-F64C-4107-87D8-5CD17FB78CFB}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4187,7 +4180,9 @@
       <c r="C8" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>323</v>
+      </c>
       <c r="F8" s="2">
         <v>7</v>
       </c>
@@ -4320,10 +4315,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73F016A4-B1D3-4DD6-A607-D0EBB6640462}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4688,24 +4683,6 @@
         <v>353</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>